<commit_message>
Deleted the insturctions on the sheet
</commit_message>
<xml_diff>
--- a/docs/unit1/3_pivot_goalseek/(Starter-Workbook)-Pre-Pivot-GoalSeek-DataV.xlsx
+++ b/docs/unit1/3_pivot_goalseek/(Starter-Workbook)-Pre-Pivot-GoalSeek-DataV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://byu-my.sharepoint.com/personal/farnssam_byu_edu/Documents/job hw keys/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CCE270\content\docs\unit1\3_pivot_goalseek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3309A7BB-351B-4422-8840-84509897D3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C95393C-93C4-4D17-A297-D5E96462B7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="-9765" windowWidth="14400" windowHeight="17400" xr2:uid="{5DED3B62-6B11-40C8-954D-550DFDBF9620}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{5DED3B62-6B11-40C8-954D-550DFDBF9620}"/>
   </bookViews>
   <sheets>
     <sheet name="Dogshow" sheetId="10" r:id="rId1"/>
@@ -34,6 +34,9 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -255,7 +258,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -646,20 +649,8 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -688,6 +679,15 @@
     <xf numFmtId="0" fontId="10" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -696,6 +696,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,187 +756,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>47627</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{519FFFF0-ACB6-45FF-8597-0A110174C720}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5467350" y="3724277"/>
-          <a:ext cx="3505200" cy="1914524"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="10000"/>
-            <a:lumOff val="90000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" algn="l" rotWithShape="0">
-            <a:prstClr val="black">
-              <a:alpha val="40000"/>
-            </a:prstClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="95000"/>
-                  <a:lumOff val="5000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Use the Data Validation tool (found under the Data tab) to limit</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="95000"/>
-                  <a:lumOff val="5000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>1.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="95000"/>
-                  <a:lumOff val="5000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> The breed of dogs (C6:C23) to the list provided </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="95000"/>
-                  <a:lumOff val="5000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>2. The judges' scores (D6:G13) to whole numbers 0 - 10</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="95000"/>
-                  <a:lumOff val="5000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>3. The winners (C28:C30) to the names of entered dogs</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1200" b="1">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="95000"/>
-                  <a:lumOff val="5000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Fill in the red chart to check your data</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="95000"/>
-                  <a:lumOff val="5000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> validation (randomly select breeds and individual judge scores).  Enter a Sum function for the total scores. Then enter the names and scores of the 1st, 2nd, and 3rd place winners. </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1004,111 +826,6 @@
             <a:rPr lang="en-US" sz="4800" b="1"/>
             <a:t>Going Fishing</a:t>
           </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{468446D1-F646-4501-8F12-F333BCC40FC9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="323850" y="1847851"/>
-          <a:ext cx="4495800" cy="2228850"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575"/>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-            <a:prstClr val="black">
-              <a:alpha val="40000"/>
-            </a:prstClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>You are out fly-fishing</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> and a huge fish just jumped high out of the water for your fly. You just happen to know the parabolic equation that all trout jumps follow which is:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>y = -(x-2)^2 + 5 </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>You want to figure out how far it jumped. Use goal seek to determine the two x values that make y = 0. Copy your answers into C28 and C29.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>As an extra curiosity you want to figure out how high the fish jumped. Use a solver to find the max y value. Copy the answer to E28.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5478,36 +5195,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9301E18-08A5-4B1A-8606-AA8CE0BAAFF7}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="13"/>
-    <col min="2" max="2" width="11.28515625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="13" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="13"/>
-    <col min="7" max="7" width="10.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="13"/>
-    <col min="10" max="10" width="16.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="9.125" style="13"/>
+    <col min="2" max="2" width="11.25" style="13" customWidth="1"/>
+    <col min="3" max="3" width="16.375" style="13" customWidth="1"/>
+    <col min="4" max="6" width="9.125" style="13"/>
+    <col min="7" max="7" width="10.75" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.125" style="13"/>
+    <col min="10" max="10" width="16.25" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:10" ht="33">
+      <c r="A1" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15">
       <c r="B5" s="19" t="s">
         <v>26</v>
       </c>
@@ -5529,11 +5246,11 @@
       <c r="I5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="B6" s="16" t="s">
         <v>34</v>
       </c>
@@ -5542,11 +5259,11 @@
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="B7" s="16" t="s">
         <v>36</v>
       </c>
@@ -5555,11 +5272,11 @@
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="B8" s="16" t="s">
         <v>38</v>
       </c>
@@ -5568,11 +5285,11 @@
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="B9" s="16" t="s">
         <v>40</v>
       </c>
@@ -5581,11 +5298,11 @@
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="B10" s="16" t="s">
         <v>42</v>
       </c>
@@ -5594,11 +5311,11 @@
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
       <c r="G10" s="18"/>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="20" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="B11" s="16" t="s">
         <v>44</v>
       </c>
@@ -5607,11 +5324,11 @@
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="B12" s="16" t="s">
         <v>46</v>
       </c>
@@ -5620,11 +5337,11 @@
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="B13" s="16" t="s">
         <v>48</v>
       </c>
@@ -5633,11 +5350,11 @@
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="B14" s="16" t="s">
         <v>50</v>
       </c>
@@ -5646,11 +5363,11 @@
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
-      <c r="J14" s="21" t="s">
+      <c r="J14" s="20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="B15" s="16" t="s">
         <v>52</v>
       </c>
@@ -5659,11 +5376,11 @@
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
-      <c r="J15" s="21" t="s">
+      <c r="J15" s="20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="B16" s="16" t="s">
         <v>54</v>
       </c>
@@ -5672,11 +5389,11 @@
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
-      <c r="J16" s="21" t="s">
+      <c r="J16" s="20" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7">
       <c r="B17" s="16" t="s">
         <v>56</v>
       </c>
@@ -5686,7 +5403,7 @@
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7">
       <c r="B18" s="16" t="s">
         <v>57</v>
       </c>
@@ -5696,7 +5413,7 @@
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7">
       <c r="B19" s="16" t="s">
         <v>58</v>
       </c>
@@ -5706,7 +5423,7 @@
       <c r="F19" s="18"/>
       <c r="G19" s="18"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7">
       <c r="B20" s="16" t="s">
         <v>59</v>
       </c>
@@ -5716,7 +5433,7 @@
       <c r="F20" s="18"/>
       <c r="G20" s="18"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7">
       <c r="B21" s="16" t="s">
         <v>60</v>
       </c>
@@ -5726,7 +5443,7 @@
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7">
       <c r="B22" s="16" t="s">
         <v>61</v>
       </c>
@@ -5736,7 +5453,7 @@
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7">
       <c r="B23" s="16" t="s">
         <v>62</v>
       </c>
@@ -5746,42 +5463,42 @@
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="34" t="s">
+    <row r="26" spans="2:7" ht="15">
+      <c r="B26" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="35"/>
-      <c r="D26" s="36"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="35"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="31"/>
-      <c r="C27" s="32" t="s">
+    <row r="27" spans="2:7">
+      <c r="B27" s="27"/>
+      <c r="C27" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="29" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="25" t="s">
+    <row r="28" spans="2:7">
+      <c r="B28" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="28"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="24"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="26" t="s">
+    <row r="29" spans="2:7">
+      <c r="B29" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="29"/>
-      <c r="D29" s="28"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="24"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="26" t="s">
+    <row r="30" spans="2:7">
+      <c r="B30" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="29"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5789,7 +5506,6 @@
     <mergeCell ref="B26:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5801,9 +5517,9 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.75" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5823,7 +5539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="2">
         <v>45658</v>
       </c>
@@ -5843,7 +5559,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" customHeight="1">
       <c r="A3" s="2">
         <v>45658</v>
       </c>
@@ -5863,7 +5579,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" customHeight="1">
       <c r="A4" s="2">
         <v>45659</v>
       </c>
@@ -5883,7 +5599,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1">
       <c r="A5" s="2">
         <v>45659</v>
       </c>
@@ -5903,7 +5619,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="2">
         <v>45660</v>
       </c>
@@ -5923,7 +5639,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="2">
         <v>45660</v>
       </c>
@@ -5943,7 +5659,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="2">
         <v>45661</v>
       </c>
@@ -5963,7 +5679,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="2">
         <v>45661</v>
       </c>
@@ -5983,7 +5699,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="2">
         <v>45662</v>
       </c>
@@ -6003,7 +5719,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="2">
         <v>45662</v>
       </c>
@@ -6023,7 +5739,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="2">
         <v>45663</v>
       </c>
@@ -6043,7 +5759,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="2">
         <v>45663</v>
       </c>
@@ -6063,7 +5779,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="2">
         <v>45664</v>
       </c>
@@ -6083,7 +5799,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="2">
         <v>45664</v>
       </c>
@@ -6103,7 +5819,7 @@
         <v>4400</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="2">
         <v>45665</v>
       </c>
@@ -6123,7 +5839,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="2">
         <v>45665</v>
       </c>
@@ -6143,7 +5859,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="2">
         <v>45666</v>
       </c>
@@ -6163,7 +5879,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="2">
         <v>45666</v>
       </c>
@@ -6183,7 +5899,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="2">
         <v>45667</v>
       </c>
@@ -6203,7 +5919,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" customHeight="1">
       <c r="A21" s="2">
         <v>45667</v>
       </c>
@@ -6223,7 +5939,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" customHeight="1">
       <c r="A22" s="2">
         <v>45668</v>
       </c>
@@ -6243,7 +5959,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" customHeight="1">
       <c r="A23" s="2">
         <v>45668</v>
       </c>
@@ -6263,7 +5979,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" customHeight="1">
       <c r="A24" s="2">
         <v>45669</v>
       </c>
@@ -6283,7 +5999,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" customHeight="1">
       <c r="A25" s="2">
         <v>45669</v>
       </c>
@@ -6303,7 +6019,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" customHeight="1">
       <c r="A26" s="2">
         <v>45670</v>
       </c>
@@ -6323,7 +6039,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" customHeight="1">
       <c r="A27" s="2">
         <v>45670</v>
       </c>
@@ -6343,7 +6059,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15" customHeight="1">
       <c r="A28" s="2">
         <v>45671</v>
       </c>
@@ -6363,7 +6079,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" customHeight="1">
       <c r="A29" s="2">
         <v>45671</v>
       </c>
@@ -6383,7 +6099,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" customHeight="1">
       <c r="A30" s="2">
         <v>45672</v>
       </c>
@@ -6403,7 +6119,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" customHeight="1">
       <c r="A31" s="2">
         <v>45672</v>
       </c>
@@ -6436,21 +6152,21 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6461,22 +6177,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93D53B0C-CC64-4005-8226-74FCED087475}">
   <dimension ref="A9:G33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="18">
       <c r="D24" s="7" t="s">
         <v>17</v>
       </c>
@@ -6485,7 +6201,7 @@
         <v>-3.6063719289991525E-5</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" ht="18">
       <c r="D25" s="7" t="s">
         <v>18</v>
       </c>
@@ -6493,7 +6209,7 @@
         <v>4.2360760415780341</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" ht="15">
       <c r="C27" s="6" t="s">
         <v>19</v>
       </c>
@@ -6501,7 +6217,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" ht="15">
       <c r="B28" s="11" t="s">
         <v>18</v>
       </c>
@@ -6511,18 +6227,18 @@
       </c>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" ht="15">
       <c r="B29" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="10"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="20" t="s">
+    <row r="32" spans="2:7" ht="15">
+      <c r="C32" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="9">
         <f>ABS(C28-C29)</f>
         <v>0</v>
@@ -6531,12 +6247,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="20" t="s">
+    <row r="33" spans="3:7" ht="15">
+      <c r="C33" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
       <c r="F33" s="12">
         <f>-((E28-2)^2)+5</f>
         <v>1</v>
@@ -6745,20 +6461,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="0fb52932-310b-4812-bc91-e280dc622503" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="0fb52932-310b-4812-bc91-e280dc622503" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6781,6 +6497,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0F68EC-7B92-4766-9A80-FE2FD3BF1281}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9B6EA4A-C2D3-4B01-A527-B52622997611}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -6795,12 +6519,4 @@
     <ds:schemaRef ds:uri="2d1d9163-36d3-4da4-a59f-c23475475079"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C0F68EC-7B92-4766-9A80-FE2FD3BF1281}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>